<commit_message>
added code for Sand Valley
</commit_message>
<xml_diff>
--- a/data/Matchups.xlsx
+++ b/data/Matchups.xlsx
@@ -8,9 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Turtle" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Ocean" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Osprey" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sand Valley" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Mammoth" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sand Valley(2)" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sedge" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Team Mac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Team Sam</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Team Sean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team JJ</t>
   </si>
   <si>
     <t xml:space="preserve">Nick Doub</t>
@@ -36,7 +37,7 @@
     <t xml:space="preserve">Sam Doub</t>
   </si>
   <si>
-    <t xml:space="preserve">Ryan Jarvis</t>
+    <t xml:space="preserve">Neil Lewnes</t>
   </si>
   <si>
     <t xml:space="preserve">JJ McKittrick</t>
@@ -48,10 +49,10 @@
     <t xml:space="preserve">Beau Wood</t>
   </si>
   <si>
-    <t xml:space="preserve">Chase Brown</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sean ODonovan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jon Toll</t>
   </si>
 </sst>
 </file>
@@ -173,10 +174,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.26"/>
@@ -234,74 +235,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.09"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -312,7 +245,75 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.09"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.09"/>
@@ -351,7 +352,74 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.77"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">

</xml_diff>